<commit_message>
Modified test methods in customer portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_2_3_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_2_3_customer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni git 13-04-23\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv2.3_Customer\14-Apr-2023(Customer)\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5765140-4F61-40C8-A0FC-D7C273AD008E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B95624-A26D-49BF-9375-DA264FF3629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -2307,26 +2307,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B5A830-0A38-42CE-920B-F809AB40B2F3}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.77734375" customWidth="1"/>
-    <col min="8" max="8" width="40.77734375" customWidth="1"/>
-    <col min="9" max="9" width="35.77734375" customWidth="1"/>
-    <col min="10" max="10" width="36.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" customWidth="1"/>
+    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" customWidth="1"/>
+    <col min="10" max="10" width="36.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2364,12 +2364,12 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>210</v>
@@ -2396,12 +2396,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>210</v>
@@ -2425,12 +2425,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>74</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>210</v>
@@ -2454,12 +2454,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="170.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>210</v>
@@ -2481,12 +2481,12 @@
       </c>
       <c r="I5" s="17"/>
     </row>
-    <row r="6" spans="1:12" ht="170.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="170.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>217</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>210</v>
@@ -2508,12 +2508,12 @@
       </c>
       <c r="I6" s="17"/>
     </row>
-    <row r="7" spans="1:12" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>219</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>210</v>
@@ -2535,12 +2535,12 @@
       </c>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:12" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="110.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>209</v>
@@ -2562,12 +2562,12 @@
       </c>
       <c r="I8" s="19"/>
     </row>
-    <row r="9" spans="1:12" ht="112.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>209</v>
@@ -2589,12 +2589,12 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="101.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="101.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>209</v>
@@ -2616,12 +2616,12 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="77.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="77.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>209</v>
@@ -2643,12 +2643,12 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="216" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>209</v>
@@ -2669,12 +2669,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>209</v>
@@ -2695,12 +2695,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>81</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>209</v>
@@ -2721,12 +2721,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>271</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>209</v>
@@ -2747,12 +2747,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>82</v>
@@ -2774,12 +2774,12 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>82</v>
@@ -2801,12 +2801,12 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>82</v>
@@ -2828,12 +2828,12 @@
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>84</v>
@@ -2855,12 +2855,12 @@
       </c>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>84</v>
@@ -2882,12 +2882,12 @@
       </c>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>84</v>
@@ -2909,12 +2909,12 @@
       </c>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>84</v>
@@ -2936,12 +2936,12 @@
       </c>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>144</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>84</v>
@@ -2963,12 +2963,12 @@
       </c>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>229</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>197</v>
@@ -2992,12 +2992,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>197</v>
@@ -3021,12 +3021,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>197</v>
@@ -3050,12 +3050,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>197</v>
@@ -3079,12 +3079,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>53</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>197</v>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="J28" s="19"/>
     </row>
-    <row r="29" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>56</v>
       </c>
@@ -3138,12 +3138,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>232</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>197</v>
@@ -3167,12 +3167,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>235</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>197</v>
@@ -3196,12 +3196,12 @@
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>197</v>
@@ -3226,12 +3226,12 @@
       </c>
       <c r="J32" s="19"/>
     </row>
-    <row r="33" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>239</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>197</v>
@@ -3256,12 +3256,12 @@
       </c>
       <c r="J33" s="19"/>
     </row>
-    <row r="34" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>197</v>
@@ -3285,12 +3285,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>268</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>197</v>
@@ -3314,12 +3314,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>197</v>
@@ -3343,12 +3343,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>243</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>197</v>
@@ -3372,12 +3372,12 @@
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>197</v>
@@ -3402,7 +3402,7 @@
       </c>
       <c r="J38" s="19"/>
     </row>
-    <row r="39" spans="1:10" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="270" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
         <v>147</v>
       </c>
@@ -3434,12 +3434,12 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="s">
         <v>253</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>198</v>
@@ -3464,12 +3464,12 @@
       </c>
       <c r="J40" s="19"/>
     </row>
-    <row r="41" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>265</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>198</v>
@@ -3494,12 +3494,12 @@
       </c>
       <c r="J41" s="19"/>
     </row>
-    <row r="42" spans="1:10" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>198</v>
@@ -3524,12 +3524,12 @@
       </c>
       <c r="J42" s="19"/>
     </row>
-    <row r="43" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>69</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>198</v>
@@ -3553,12 +3553,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>251</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>198</v>
@@ -3582,12 +3582,12 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>198</v>
@@ -3611,12 +3611,12 @@
         <v>255</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>151</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>198</v>
@@ -3640,12 +3640,12 @@
         <v>273</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>198</v>
@@ -3669,12 +3669,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>154</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>198</v>
@@ -3698,12 +3698,12 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>258</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>198</v>
@@ -3727,12 +3727,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>198</v>
@@ -3756,12 +3756,12 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" ht="285" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>198</v>
@@ -3785,12 +3785,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>85</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>199</v>
@@ -3814,12 +3814,12 @@
         <v>245</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>197</v>
@@ -3843,12 +3843,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>89</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>200</v>
@@ -3872,12 +3872,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>91</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>82</v>
@@ -3899,12 +3899,12 @@
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>84</v>
@@ -3926,12 +3926,12 @@
       </c>
       <c r="I56" s="12"/>
     </row>
-    <row r="57" spans="1:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>92</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>201</v>
@@ -3956,12 +3956,12 @@
       </c>
       <c r="J57" s="19"/>
     </row>
-    <row r="58" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>94</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>201</v>
@@ -3994,12 +3994,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>95</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>201</v>
@@ -4032,12 +4032,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>96</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>201</v>
@@ -4062,12 +4062,12 @@
       </c>
       <c r="J60" s="28"/>
     </row>
-    <row r="61" spans="1:12" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>97</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>201</v>
@@ -4092,12 +4092,12 @@
       </c>
       <c r="J61" s="28"/>
     </row>
-    <row r="62" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>98</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>201</v>
@@ -4130,12 +4130,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>99</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>201</v>
@@ -4168,7 +4168,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
         <v>100</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
         <v>102</v>
       </c>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="J65" s="28"/>
     </row>
-    <row r="66" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
         <v>103</v>
       </c>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="J66" s="28"/>
     </row>
-    <row r="67" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
         <v>104</v>
       </c>
@@ -4289,12 +4289,12 @@
         <v>274</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
         <v>106</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>202</v>
@@ -4318,12 +4318,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
         <v>107</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C69" s="26" t="s">
         <v>202</v>
@@ -4347,12 +4347,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
         <v>108</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C70" s="26" t="s">
         <v>202</v>
@@ -4379,12 +4379,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
         <v>110</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C71" s="26" t="s">
         <v>202</v>
@@ -4409,12 +4409,12 @@
       </c>
       <c r="J71" s="28"/>
     </row>
-    <row r="72" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
         <v>111</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C72" s="26" t="s">
         <v>202</v>
@@ -4439,12 +4439,12 @@
       </c>
       <c r="J72" s="28"/>
     </row>
-    <row r="73" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
         <v>263</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C73" s="26" t="s">
         <v>202</v>
@@ -4469,12 +4469,12 @@
       </c>
       <c r="J73" s="28"/>
     </row>
-    <row r="74" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
         <v>264</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C74" s="26" t="s">
         <v>202</v>
@@ -4499,12 +4499,12 @@
       </c>
       <c r="J74" s="28"/>
     </row>
-    <row r="75" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>112</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C75" s="26" t="s">
         <v>203</v>
@@ -4531,12 +4531,12 @@
         <v>278</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>290</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C76" s="26" t="s">
         <v>203</v>
@@ -4561,7 +4561,7 @@
       </c>
       <c r="J76" s="19"/>
     </row>
-    <row r="77" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>114</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>115</v>
       </c>
@@ -4619,12 +4619,12 @@
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>294</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79" s="26" t="s">
         <v>203</v>
@@ -4648,7 +4648,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="273.60000000000002" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>116</v>
       </c>
@@ -4680,7 +4680,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
         <v>118</v>
       </c>
@@ -4709,12 +4709,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>119</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>205</v>
@@ -4738,12 +4738,12 @@
         <v>280</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>282</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>286</v>
@@ -4767,12 +4767,12 @@
         <v>287</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>283</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>286</v>
@@ -4796,12 +4796,12 @@
         <v>289</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>284</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>286</v>
@@ -4825,12 +4825,12 @@
         <v>288</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>121</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>206</v>
@@ -4854,12 +4854,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>123</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>206</v>
@@ -4883,7 +4883,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A88" s="32" t="s">
         <v>125</v>
       </c>
@@ -4912,12 +4912,12 @@
         <v>281</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
         <v>127</v>
       </c>
       <c r="B89" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>197</v>
@@ -4941,7 +4941,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>129</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>132</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>133</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>135</v>
       </c>
@@ -5086,7 +5086,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>137</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>138</v>
       </c>
@@ -5144,12 +5144,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>139</v>
       </c>
       <c r="B97" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C97" s="20" t="s">
         <v>197</v>
@@ -5173,12 +5173,12 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>249</v>
       </c>
       <c r="B98" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C98" s="20" t="s">
         <v>197</v>
@@ -5202,12 +5202,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>141</v>
       </c>
       <c r="B99" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C99" s="20" t="s">
         <v>197</v>
@@ -5231,12 +5231,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>142</v>
       </c>
       <c r="B100" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C100" s="20" t="s">
         <v>197</v>
@@ -5260,12 +5260,12 @@
         <v>193</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>42</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>197</v>
@@ -5290,12 +5290,12 @@
       </c>
       <c r="J101" s="19"/>
     </row>
-    <row r="102" spans="1:10" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>212</v>
       </c>
       <c r="B102" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>213</v>
@@ -5356,14 +5356,14 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -5379,12 +5379,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Developed the page classes and components for coyni3.0
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/TestScript_2_3_customer.xlsx
+++ b/Mobile/coyni_mobile/resources/TestScript_2_3_customer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv2.3_Customer\14-Apr-2023(Customer)\coyni-automation\Mobile\coyni_mobile\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coyni_V3.0_Personal\18-May-2023_V3.0\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B95624-A26D-49BF-9375-DA264FF3629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736F87FE-C4E6-46C5-B0EC-4C2B7E79CDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5C6B0436-5574-461E-BCCD-7B4ECDABB879}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="303">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -331,24 +331,10 @@
     <t>Verify Add Credit Card With Invalid Data</t>
   </si>
   <si>
-    <t>Verify SignUp with valid credentials by adding DebitCard, uncheck Address</t>
-  </si>
-  <si>
     <t>Verify SignUp with valid credentials and Skip Adding cards</t>
   </si>
   <si>
     <t>Verify SignUp with valid credentials by adding CreditCard, check Address</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.CustomerProfileTest,
-testAddAddressFromDashboard,
--paddressLine1,
--paddreddLine2,
--pcity,
--pstate,
--pzipCode,
--pcountryName,
--paddressAddedPage</t>
   </si>
   <si>
     <t>coyni_mobile.tests.SignUpTest,
@@ -1090,57 +1076,6 @@
 -pconfirmPassword,
 -pexpMessage,
 -pcode</t>
-  </si>
-  <si>
-    <t>coyni_mobile.tests.SignUpTest,
-testSignUpTwoDotThree,
--pcreateAccount,
--pfirstName,
--plastName,
--pemail,
--pphoneNumber,
--ppassword,
--pconfirmPassword,
--pphoneVerificationPageHeading,
--pphoneDescription,
--pcode,
--pemailVerificationPageHeading,
--pemailDescription,
--ptoastMessage,
--ptermsOfServicePageHeading,
--pprivacyPolicyPageHeading,
--psecureYourAccountPageHeading,
--psecureAccountDescription,
--pchoosePinHeading,
--ppin,
--pconfirmPinHeading,
--penableTouchIdPageHeading,
--pidDescription,
--pcreateAccountPageHeading,
--paccountDescription,
--pvalidateAddCreditOrDebit,
--pcardDetailsHeading,
--pnameOnCard,
--pcardNumber,
--pcardExp,
--pcvvOrCVC,
--paddAddressHeading,
--paddressLine1,
--paddreddLine2,
--pcity,
--pstate,
--pzipCode,
--pcountryName,
--pvalidateSaveAddress,
--ppreAuthHeading,
--ppreAuthDescription,
--ppreAuthiAmount,
--psuccessHeading,
--psuccessDescription,
--pvalidateSkip,
--pviewAddAddress,
--pviewBuyToken,
--pviewAddPayment</t>
   </si>
   <si>
     <t>coyni_mobile.tests.SignUpTest,
@@ -1805,6 +1740,13 @@
   </si>
   <si>
     <t>forgotpin-Invalid</t>
+  </si>
+  <si>
+    <t>coyni_mobile.tests.SignUpTest,
+testSignUp</t>
+  </si>
+  <si>
+    <t>Verify SignUp with valid credentials</t>
   </si>
 </sst>
 </file>
@@ -2308,7 +2250,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,24 +2297,24 @@
         <v>14</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>73</v>
+        <v>302</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>8</v>
@@ -2387,24 +2329,20 @@
         <v>30</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>45</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:12" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>8</v>
@@ -2419,7 +2357,7 @@
         <v>30</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>45</v>
@@ -2427,13 +2365,13 @@
     </row>
     <row r="4" spans="1:12" ht="409.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>8</v>
@@ -2448,7 +2386,7 @@
         <v>30</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>45</v>
@@ -2462,7 +2400,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D5" s="22" t="s">
         <v>10</v>
@@ -2471,25 +2409,25 @@
         <v>9</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G5" s="24" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:12" ht="170.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>10</v>
@@ -2504,19 +2442,19 @@
         <v>30</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:12" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>10</v>
@@ -2531,7 +2469,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I7" s="17"/>
     </row>
@@ -2543,7 +2481,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>8</v>
@@ -2558,7 +2496,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I8" s="19"/>
     </row>
@@ -2570,7 +2508,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>10</v>
@@ -2585,7 +2523,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I9" s="3"/>
     </row>
@@ -2597,7 +2535,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
@@ -2612,7 +2550,7 @@
         <v>24</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I10" s="3"/>
     </row>
@@ -2624,7 +2562,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
@@ -2645,13 +2583,13 @@
     </row>
     <row r="12" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -2666,7 +2604,7 @@
         <v>49</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
@@ -2677,7 +2615,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -2697,13 +2635,13 @@
     </row>
     <row r="14" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -2715,7 +2653,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>52</v>
@@ -2723,13 +2661,13 @@
     </row>
     <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -2741,10 +2679,10 @@
         <v>9</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="165" x14ac:dyDescent="0.25">
@@ -2755,7 +2693,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -2782,7 +2720,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>10</v>
@@ -2794,7 +2732,7 @@
         <v>67</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>36</v>
@@ -2809,7 +2747,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
@@ -2821,10 +2759,10 @@
         <v>9</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -2836,7 +2774,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>8</v>
@@ -2848,10 +2786,10 @@
         <v>9</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I19" s="12"/>
     </row>
@@ -2863,7 +2801,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>10</v>
@@ -2875,10 +2813,10 @@
         <v>22</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I20" s="12"/>
     </row>
@@ -2890,7 +2828,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>8</v>
@@ -2902,10 +2840,10 @@
         <v>9</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="I21" s="12"/>
     </row>
@@ -2917,7 +2855,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>10</v>
@@ -2929,22 +2867,22 @@
         <v>9</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>10</v>
@@ -2956,22 +2894,22 @@
         <v>9</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>10</v>
@@ -2983,13 +2921,13 @@
         <v>9</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -3000,7 +2938,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>10</v>
@@ -3018,7 +2956,7 @@
         <v>28</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -3029,7 +2967,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>10</v>
@@ -3058,7 +2996,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>10</v>
@@ -3076,7 +3014,7 @@
         <v>28</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -3087,7 +3025,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D28" s="20" t="s">
         <v>10</v>
@@ -3117,7 +3055,7 @@
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D29" s="20" t="s">
         <v>10</v>
@@ -3140,13 +3078,13 @@
     </row>
     <row r="30" spans="1:10" ht="225" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>10</v>
@@ -3158,24 +3096,24 @@
         <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H30" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>10</v>
@@ -3187,13 +3125,13 @@
         <v>9</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="H31" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3204,7 +3142,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>10</v>
@@ -3222,19 +3160,19 @@
         <v>28</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J32" s="19"/>
     </row>
     <row r="33" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>10</v>
@@ -3246,13 +3184,13 @@
         <v>9</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="H33" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="J33" s="19"/>
     </row>
@@ -3264,7 +3202,7 @@
         <v>12</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>10</v>
@@ -3282,18 +3220,18 @@
         <v>28</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>10</v>
@@ -3311,7 +3249,7 @@
         <v>28</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="225" x14ac:dyDescent="0.25">
@@ -3322,7 +3260,7 @@
         <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>10</v>
@@ -3340,18 +3278,18 @@
         <v>28</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>10</v>
@@ -3369,7 +3307,7 @@
         <v>28</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="210" x14ac:dyDescent="0.25">
@@ -3380,7 +3318,7 @@
         <v>12</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>10</v>
@@ -3404,13 +3342,13 @@
     </row>
     <row r="39" spans="1:10" ht="270" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>10</v>
@@ -3422,27 +3360,27 @@
         <v>47</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>8</v>
@@ -3454,25 +3392,25 @@
         <v>9</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H40" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>10</v>
@@ -3484,13 +3422,13 @@
         <v>47</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H41" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J41" s="19"/>
     </row>
@@ -3502,7 +3440,7 @@
         <v>12</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>10</v>
@@ -3514,13 +3452,13 @@
         <v>9</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H42" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J42" s="19"/>
     </row>
@@ -3532,7 +3470,7 @@
         <v>12</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>10</v>
@@ -3544,7 +3482,7 @@
         <v>9</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H43" s="11" t="s">
         <v>28</v>
@@ -3555,13 +3493,13 @@
     </row>
     <row r="44" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B44" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>10</v>
@@ -3573,13 +3511,13 @@
         <v>67</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H44" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -3590,7 +3528,7 @@
         <v>12</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>10</v>
@@ -3602,24 +3540,24 @@
         <v>9</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H45" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B46" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>10</v>
@@ -3628,27 +3566,27 @@
         <v>9</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>10</v>
@@ -3660,24 +3598,24 @@
         <v>9</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>10</v>
@@ -3689,24 +3627,24 @@
         <v>9</v>
       </c>
       <c r="G48" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="8" t="s">
         <v>153</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="300" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B49" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>10</v>
@@ -3718,24 +3656,24 @@
         <v>67</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H49" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B50" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D50" s="20" t="s">
         <v>10</v>
@@ -3747,13 +3685,13 @@
         <v>9</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="285" x14ac:dyDescent="0.25">
@@ -3764,7 +3702,7 @@
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D51" s="20" t="s">
         <v>10</v>
@@ -3773,27 +3711,27 @@
         <v>9</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H51" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B52" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D52" s="20" t="s">
         <v>10</v>
@@ -3802,27 +3740,27 @@
         <v>9</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H52" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B53" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D53" s="20" t="s">
         <v>10</v>
@@ -3834,24 +3772,24 @@
         <v>9</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B54" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D54" s="20" t="s">
         <v>10</v>
@@ -3863,24 +3801,24 @@
         <v>9</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H54" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B55" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>10</v>
@@ -3895,7 +3833,7 @@
         <v>16</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I55" s="1"/>
     </row>
@@ -3907,7 +3845,7 @@
         <v>12</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D56" s="20" t="s">
         <v>10</v>
@@ -3922,19 +3860,19 @@
         <v>20</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I56" s="12"/>
     </row>
     <row r="57" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B57" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>10</v>
@@ -3946,25 +3884,25 @@
         <v>9</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H57" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I57" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J57" s="19"/>
     </row>
     <row r="58" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B58" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D58" s="20" t="s">
         <v>10</v>
@@ -3976,33 +3914,33 @@
         <v>9</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H58" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I58" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J58" s="19" t="s">
         <v>45</v>
       </c>
       <c r="K58" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L58" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B59" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D59" s="20" t="s">
         <v>10</v>
@@ -4014,33 +3952,33 @@
         <v>9</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H59" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I59" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J59" s="19" t="s">
         <v>45</v>
       </c>
       <c r="K59" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="L59" s="28" t="s">
         <v>164</v>
-      </c>
-      <c r="L59" s="28" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B60" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D60" s="20" t="s">
         <v>10</v>
@@ -4052,25 +3990,25 @@
         <v>9</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H60" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I60" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J60" s="28"/>
     </row>
     <row r="61" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B61" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D61" s="20" t="s">
         <v>10</v>
@@ -4082,25 +4020,25 @@
         <v>9</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H61" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I61" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J61" s="28"/>
     </row>
     <row r="62" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B62" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>10</v>
@@ -4112,33 +4050,33 @@
         <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H62" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I62" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J62" s="19" t="s">
         <v>45</v>
       </c>
       <c r="K62" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L62" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B63" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>10</v>
@@ -4150,33 +4088,33 @@
         <v>9</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H63" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I63" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J63" s="19" t="s">
         <v>45</v>
       </c>
       <c r="K63" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L63" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="225" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B64" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D64" s="20" t="s">
         <v>10</v>
@@ -4188,24 +4126,24 @@
         <v>9</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I64" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B65" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C65" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D65" s="20" t="s">
         <v>10</v>
@@ -4217,25 +4155,25 @@
         <v>47</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H65" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I65" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J65" s="28"/>
     </row>
     <row r="66" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B66" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D66" s="20" t="s">
         <v>10</v>
@@ -4247,25 +4185,25 @@
         <v>9</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H66" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I66" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J66" s="28"/>
     </row>
     <row r="67" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A67" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B67" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D67" s="20" t="s">
         <v>10</v>
@@ -4277,27 +4215,27 @@
         <v>9</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H67" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I67" s="19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J67" s="19" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B68" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D68" s="20" t="s">
         <v>10</v>
@@ -4309,24 +4247,24 @@
         <v>47</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H68" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I68" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B69" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D69" s="20" t="s">
         <v>10</v>
@@ -4338,24 +4276,24 @@
         <v>9</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H69" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I69" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A70" s="29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B70" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D70" s="20" t="s">
         <v>10</v>
@@ -4367,27 +4305,27 @@
         <v>9</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H70" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I70" s="19" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J70" s="19" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B71" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C71" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D71" s="20" t="s">
         <v>10</v>
@@ -4399,25 +4337,25 @@
         <v>47</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H71" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I71" s="19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J71" s="28"/>
     </row>
     <row r="72" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A72" s="29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B72" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C72" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>10</v>
@@ -4429,25 +4367,25 @@
         <v>9</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H72" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J72" s="28"/>
     </row>
     <row r="73" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B73" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C73" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>10</v>
@@ -4459,25 +4397,25 @@
         <v>9</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H73" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I73" s="19" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J73" s="28"/>
     </row>
     <row r="74" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A74" s="29" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B74" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>10</v>
@@ -4489,25 +4427,25 @@
         <v>9</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H74" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I74" s="19" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="J74" s="28"/>
     </row>
     <row r="75" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B75" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C75" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>10</v>
@@ -4519,57 +4457,57 @@
         <v>9</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H75" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I75" s="19" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J75" s="19" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>287</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B76" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C76" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>293</v>
-      </c>
       <c r="H76" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I76" s="19" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J76" s="19"/>
     </row>
     <row r="77" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B77" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C77" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>10</v>
@@ -4581,24 +4519,24 @@
         <v>22</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H77" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I77" s="19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B78" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C78" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>10</v>
@@ -4610,24 +4548,24 @@
         <v>9</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H78" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I78" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B79" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C79" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>10</v>
@@ -4639,24 +4577,24 @@
         <v>9</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H79" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I79" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B80" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D80" s="20" t="s">
         <v>10</v>
@@ -4668,27 +4606,27 @@
         <v>9</v>
       </c>
       <c r="G80" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H80" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J80" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B81" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D81" s="20" t="s">
         <v>10</v>
@@ -4700,24 +4638,24 @@
         <v>9</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H81" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I81" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="I81" s="8" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B82" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D82" s="20" t="s">
         <v>10</v>
@@ -4729,24 +4667,24 @@
         <v>9</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H82" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I82" s="19" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B83" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D83" s="20" t="s">
         <v>10</v>
@@ -4758,53 +4696,53 @@
         <v>22</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H83" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>280</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B84" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C84" s="3" t="s">
+      <c r="D84" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H84" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I84" s="19" t="s">
         <v>286</v>
-      </c>
-      <c r="D84" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="H84" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I84" s="19" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B85" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>10</v>
@@ -4816,24 +4754,24 @@
         <v>9</v>
       </c>
       <c r="G85" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I85" s="19" t="s">
         <v>285</v>
-      </c>
-      <c r="H85" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I85" s="19" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B86" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D86" s="20" t="s">
         <v>10</v>
@@ -4845,24 +4783,24 @@
         <v>9</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H86" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I86" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B87" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D87" s="20" t="s">
         <v>10</v>
@@ -4874,24 +4812,24 @@
         <v>9</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H87" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I87" s="19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A88" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B88" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D88" s="20" t="s">
         <v>10</v>
@@ -4903,24 +4841,24 @@
         <v>9</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H88" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I88" s="19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B89" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D89" s="20" t="s">
         <v>10</v>
@@ -4932,24 +4870,24 @@
         <v>9</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I89" s="19" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B90" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D90" s="20" t="s">
         <v>10</v>
@@ -4961,24 +4899,24 @@
         <v>9</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H90" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I90" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B91" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D91" s="20" t="s">
         <v>10</v>
@@ -4990,24 +4928,24 @@
         <v>9</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H91" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I91" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B92" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D92" s="20" t="s">
         <v>10</v>
@@ -5019,24 +4957,24 @@
         <v>9</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H92" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I92" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B93" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D93" s="20" t="s">
         <v>10</v>
@@ -5048,24 +4986,24 @@
         <v>9</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H93" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I93" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="270" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B94" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D94" s="20" t="s">
         <v>10</v>
@@ -5077,24 +5015,24 @@
         <v>47</v>
       </c>
       <c r="G94" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H94" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="210" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B95" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D95" s="20" t="s">
         <v>10</v>
@@ -5103,27 +5041,27 @@
         <v>9</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G95" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B96" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D96" s="20" t="s">
         <v>10</v>
@@ -5135,24 +5073,24 @@
         <v>9</v>
       </c>
       <c r="G96" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B97" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D97" s="20" t="s">
         <v>10</v>
@@ -5164,24 +5102,24 @@
         <v>9</v>
       </c>
       <c r="G97" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H97" s="8" t="s">
         <v>28</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B98" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D98" s="20" t="s">
         <v>10</v>
@@ -5193,24 +5131,24 @@
         <v>9</v>
       </c>
       <c r="G98" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H98" s="8" t="s">
         <v>28</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B99" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D99" s="20" t="s">
         <v>10</v>
@@ -5222,24 +5160,24 @@
         <v>9</v>
       </c>
       <c r="G99" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H99" s="8" t="s">
         <v>28</v>
       </c>
       <c r="I99" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B100" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D100" s="20" t="s">
         <v>10</v>
@@ -5251,13 +5189,13 @@
         <v>9</v>
       </c>
       <c r="G100" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H100" s="8" t="s">
         <v>28</v>
       </c>
       <c r="I100" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
@@ -5268,7 +5206,7 @@
         <v>12</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D101" s="20" t="s">
         <v>10</v>
@@ -5292,13 +5230,13 @@
     </row>
     <row r="102" spans="1:10" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B102" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D102" s="20" t="s">
         <v>8</v>
@@ -5310,13 +5248,13 @@
         <v>9</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H102" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I102" s="19" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>